<commit_message>
Added other user for myself
</commit_message>
<xml_diff>
--- a/Campus_SV_New.xlsx
+++ b/Campus_SV_New.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sebastian 1/PycharmProjects/Campus_San_Val_Repo1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA49E036-C44C-3A4B-80A1-D84A5C7E3A5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E7B54F-D17D-8746-A24C-C1BACC5B77E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="500" windowWidth="21900" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="284">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1157,7 +1157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1197,6 +1197,9 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1415,16 +1418,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AW70"/>
+  <dimension ref="A1:AW71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="12" width="18.83203125" customWidth="1"/>
+    <col min="1" max="6" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.5" customWidth="1"/>
+    <col min="8" max="12" width="18.83203125" customWidth="1"/>
     <col min="13" max="13" width="27.1640625" customWidth="1"/>
     <col min="14" max="14" width="6.5" customWidth="1"/>
     <col min="15" max="15" width="54.1640625" customWidth="1"/>
@@ -1452,7 +1457,7 @@
     <col min="43" max="49" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="112" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:49" ht="228" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1474,7 +1479,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="37" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -10784,6 +10789,137 @@
         <v>-1</v>
       </c>
     </row>
+    <row r="71" spans="1:49" ht="13" x14ac:dyDescent="0.15">
+      <c r="A71" s="2">
+        <v>45340.566548159724</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="E71" s="3">
+        <v>6241579275</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I71" s="3">
+        <v>2</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L71" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M71" s="3">
+        <v>-2</v>
+      </c>
+      <c r="N71" s="3">
+        <v>2</v>
+      </c>
+      <c r="O71" s="3">
+        <v>-1</v>
+      </c>
+      <c r="P71" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q71" s="3">
+        <v>-2</v>
+      </c>
+      <c r="R71" s="3">
+        <v>2</v>
+      </c>
+      <c r="S71" s="3">
+        <v>-2</v>
+      </c>
+      <c r="T71" s="3">
+        <v>0</v>
+      </c>
+      <c r="U71" s="3">
+        <v>1</v>
+      </c>
+      <c r="V71" s="3">
+        <v>1</v>
+      </c>
+      <c r="W71" s="3">
+        <v>1</v>
+      </c>
+      <c r="X71" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y71" s="3">
+        <v>1</v>
+      </c>
+      <c r="Z71" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA71" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB71" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC71" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AD71" s="3">
+        <v>2</v>
+      </c>
+      <c r="AE71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF71" s="3">
+        <v>2</v>
+      </c>
+      <c r="AG71" s="3">
+        <v>2</v>
+      </c>
+      <c r="AH71" s="3">
+        <v>2</v>
+      </c>
+      <c r="AI71" s="3">
+        <v>-2</v>
+      </c>
+      <c r="AJ71" s="3">
+        <v>2</v>
+      </c>
+      <c r="AK71" s="3">
+        <v>2</v>
+      </c>
+      <c r="AL71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AM71" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AN71" s="3">
+        <v>-1</v>
+      </c>
+      <c r="AO71" s="3">
+        <v>0</v>
+      </c>
+      <c r="AP71" s="3">
+        <v>-2</v>
+      </c>
+      <c r="AQ71" s="3">
+        <v>-1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Eliminated myself from excel
</commit_message>
<xml_diff>
--- a/Campus_SV_New.xlsx
+++ b/Campus_SV_New.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sebastian 1/PycharmProjects/Campus_San_Val_Repo1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46642007-5679-0145-9003-72EF430DA329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{881189AC-678E-4D4A-87FB-2ACEC111AA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="660" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="281">
   <si>
     <t>Timestamp</t>
   </si>
@@ -994,15 +994,6 @@
   </si>
   <si>
     <t>a.glez_18</t>
-  </si>
-  <si>
-    <t>sebysurfer@gmail.com</t>
-  </si>
-  <si>
-    <t>Sebastián W</t>
-  </si>
-  <si>
-    <t>sebysurfer2003</t>
   </si>
 </sst>
 </file>
@@ -1418,10 +1409,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AW71"/>
+  <dimension ref="A1:AW69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
@@ -10658,268 +10649,6 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="70" spans="1:49" ht="13" x14ac:dyDescent="0.15">
-      <c r="A70" s="2">
-        <v>45340.566548159724</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E70" s="3">
-        <v>6241579275</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H70" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I70" s="3">
-        <v>2</v>
-      </c>
-      <c r="J70" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L70" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M70" s="3">
-        <v>-2</v>
-      </c>
-      <c r="N70" s="3">
-        <v>2</v>
-      </c>
-      <c r="O70" s="3">
-        <v>-1</v>
-      </c>
-      <c r="P70" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q70" s="3">
-        <v>-2</v>
-      </c>
-      <c r="R70" s="3">
-        <v>2</v>
-      </c>
-      <c r="S70" s="3">
-        <v>-2</v>
-      </c>
-      <c r="T70" s="3">
-        <v>0</v>
-      </c>
-      <c r="U70" s="3">
-        <v>1</v>
-      </c>
-      <c r="V70" s="3">
-        <v>1</v>
-      </c>
-      <c r="W70" s="3">
-        <v>1</v>
-      </c>
-      <c r="X70" s="3">
-        <v>2</v>
-      </c>
-      <c r="Y70" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z70" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA70" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB70" s="3">
-        <v>2</v>
-      </c>
-      <c r="AC70" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AD70" s="3">
-        <v>2</v>
-      </c>
-      <c r="AE70" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF70" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG70" s="3">
-        <v>2</v>
-      </c>
-      <c r="AH70" s="3">
-        <v>2</v>
-      </c>
-      <c r="AI70" s="3">
-        <v>-2</v>
-      </c>
-      <c r="AJ70" s="3">
-        <v>2</v>
-      </c>
-      <c r="AK70" s="3">
-        <v>2</v>
-      </c>
-      <c r="AL70" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM70" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AN70" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AO70" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP70" s="3">
-        <v>-2</v>
-      </c>
-      <c r="AQ70" s="3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:49" ht="13" x14ac:dyDescent="0.15">
-      <c r="A71" s="2">
-        <v>45340.566548159724</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="E71" s="3">
-        <v>6241579275</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H71" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I71" s="3">
-        <v>2</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="L71" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="M71" s="3">
-        <v>-2</v>
-      </c>
-      <c r="N71" s="3">
-        <v>2</v>
-      </c>
-      <c r="O71" s="3">
-        <v>-1</v>
-      </c>
-      <c r="P71" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q71" s="3">
-        <v>-2</v>
-      </c>
-      <c r="R71" s="3">
-        <v>2</v>
-      </c>
-      <c r="S71" s="3">
-        <v>-2</v>
-      </c>
-      <c r="T71" s="3">
-        <v>0</v>
-      </c>
-      <c r="U71" s="3">
-        <v>1</v>
-      </c>
-      <c r="V71" s="3">
-        <v>1</v>
-      </c>
-      <c r="W71" s="3">
-        <v>1</v>
-      </c>
-      <c r="X71" s="3">
-        <v>2</v>
-      </c>
-      <c r="Y71" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z71" s="3">
-        <v>2</v>
-      </c>
-      <c r="AA71" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB71" s="3">
-        <v>2</v>
-      </c>
-      <c r="AC71" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AD71" s="3">
-        <v>2</v>
-      </c>
-      <c r="AE71" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF71" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG71" s="3">
-        <v>2</v>
-      </c>
-      <c r="AH71" s="3">
-        <v>2</v>
-      </c>
-      <c r="AI71" s="3">
-        <v>-2</v>
-      </c>
-      <c r="AJ71" s="3">
-        <v>2</v>
-      </c>
-      <c r="AK71" s="3">
-        <v>2</v>
-      </c>
-      <c r="AL71" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM71" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AN71" s="3">
-        <v>-1</v>
-      </c>
-      <c r="AO71" s="3">
-        <v>0</v>
-      </c>
-      <c r="AP71" s="3">
-        <v>-2</v>
-      </c>
-      <c r="AQ71" s="3">
-        <v>-1</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>